<commit_message>
one section to go
</commit_message>
<xml_diff>
--- a/data/harpur-lang.xlsx
+++ b/data/harpur-lang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/falk/github/articles/harpur-dunlop-wulatji/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4433BC96-8610-F04D-A2B7-7F24647B1F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ED9664-FC8B-5949-8054-8990F8707162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{FC4BB2E0-FBC5-FD45-B13A-126658919CD1}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{FC4BB2E0-FBC5-FD45-B13A-126658919CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -620,10 +620,10 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>